<commit_message>
Add data preview enhancements and dark mode improvements
Features:
- Sticky navigation bar for better UX
- Data preview shows first 5 and last 5 rows in separate tables
- Compact inline column names with numbered badges
- Dark mode color adjustments for better visibility

Changes:
- Made nav bar sticky to top with z-index 1000
- Modified backend to send first 5 + last 5 rows preview
- Restructured DataDisplay to show two separate tables
- Changed column names from grid to inline flex layout
- Added theme-aware colors (#667eea light, #172E5C dark)
- Updated table headers and badges for dark mode
- Created TODO.md with data type validation feature plan

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample_data/large_dataset.xlsx
+++ b/sample_data/large_dataset.xlsx
@@ -561,11 +561,6 @@
           <t>736938</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>buddhism</t>
@@ -858,9 +853,6 @@
         <is>
           <t>islam</t>
         </is>
-      </c>
-      <c r="D6">
-        <v>40</v>
       </c>
       <c r="E6">
         <v>92.90000000000001</v>

</xml_diff>